<commit_message>
updated sorting by matrix_number
</commit_message>
<xml_diff>
--- a/sandbox/Yield Matrix-backup.xlsx
+++ b/sandbox/Yield Matrix-backup.xlsx
@@ -668,20 +668,15 @@
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="17" style="1" customWidth="1"/>
-    <col min="10" max="11" width="18.28515625" customWidth="1"/>
-    <col min="12" max="17" width="21.140625" customWidth="1"/>
-    <col min="18" max="18" width="29.5703125" customWidth="1"/>
-    <col min="19" max="19" width="11.140625" customWidth="1"/>
-    <col min="20" max="20" width="14.85546875" customWidth="1"/>
+    <col min="2" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10" max="20" width="15.7109375" customWidth="1"/>
     <col min="21" max="21" width="4.28515625" customWidth="1"/>
     <col min="22" max="22" width="10.42578125" customWidth="1"/>
     <col min="23" max="24" width="10.7109375" customWidth="1"/>

</xml_diff>